<commit_message>
- add question grouping for color scale - color_scale with str_wrap - longer long_palette
</commit_message>
<xml_diff>
--- a/inst/extdata/mock_seged.xlsx
+++ b/inst/extdata/mock_seged.xlsx
@@ -1,20 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbali\Documents\Projektek\MR_Pres_Auto\V2\177_TAPADULT_250626\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbali\Documents\Projektek\custom_packages\rflib\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{518FB6E7-44DB-4A61-AA5E-FC0C5142543A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81AA011C-19BA-4FC2-ACBA-A667A6A8A49D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3465" yWindow="3465" windowWidth="21600" windowHeight="11295" xr2:uid="{912F9847-1AF1-481B-9E06-52B0F0841963}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{912F9847-1AF1-481B-9E06-52B0F0841963}"/>
   </bookViews>
   <sheets>
-    <sheet name="Munka1" sheetId="1" r:id="rId1"/>
-    <sheet name="Munka2" sheetId="2" r:id="rId2"/>
+    <sheet name="Types" sheetId="1" r:id="rId1"/>
+    <sheet name="Likert" sheetId="2" r:id="rId2"/>
+    <sheet name="AnswerGroups" sheetId="4" r:id="rId3"/>
+    <sheet name="Forrás" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="34">
   <si>
     <t>kerdes_szam</t>
   </si>
@@ -115,6 +117,30 @@
   </si>
   <si>
     <t>table_rev</t>
+  </si>
+  <si>
+    <t>first_label</t>
+  </si>
+  <si>
+    <t>last_label</t>
+  </si>
+  <si>
+    <t>Egyáltalán nem</t>
+  </si>
+  <si>
+    <t>Teljes mértékben</t>
+  </si>
+  <si>
+    <t>question_id</t>
+  </si>
+  <si>
+    <t>group1</t>
+  </si>
+  <si>
+    <t>group2</t>
+  </si>
+  <si>
+    <t>group3</t>
   </si>
 </sst>
 </file>
@@ -495,17 +521,15 @@
   <sheetPr codeName="Munka1"/>
   <dimension ref="A1:D39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -519,7 +543,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -530,7 +554,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -541,7 +565,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -552,7 +576,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -563,7 +587,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -574,7 +598,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -585,7 +609,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -596,7 +620,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -607,7 +631,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -618,7 +642,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -629,7 +653,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -640,7 +664,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -651,7 +675,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -662,7 +686,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -673,7 +697,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -684,7 +708,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -695,7 +719,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -706,7 +730,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -717,57 +741,57 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="2"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="2"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="2"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="2"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="2"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="2"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="2"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="2"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="2"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C32" s="1"/>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="2"/>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C34" s="1"/>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="2"/>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="2"/>
       <c r="C36" s="1"/>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="2"/>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" s="2"/>
       <c r="C38" s="1"/>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" s="2"/>
     </row>
   </sheetData>
@@ -779,21 +803,128 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{423F8F39-F8DF-4455-9B2B-14DDF0D8BEA8}">
   <sheetPr codeName="Munka2"/>
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20" customWidth="1"/>
+    <col min="3" max="3" width="25.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="2">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="2"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="2"/>
+      <c r="B5" s="1"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="2"/>
+      <c r="B6" s="1"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="2"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{662A3F05-A97A-4276-B2AE-1E6E7FF6A7AA}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{766E6A2A-7957-469A-B7BA-1CA94A470C55}">
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="32.42578125" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" customWidth="1"/>
+    <col min="1" max="1" width="32.44140625" customWidth="1"/>
+    <col min="2" max="2" width="18.88671875" customWidth="1"/>
     <col min="3" max="3" width="20" customWidth="1"/>
-    <col min="4" max="4" width="25.85546875" customWidth="1"/>
+    <col min="4" max="4" width="25.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -807,87 +938,87 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>20</v>
       </c>

</xml_diff>

<commit_message>
Implement lazy loading functionality for survey plotting
- Introduced lazy loading for plot creation in survey questions to enhance memory efficiency and performance.
- Updated `survey_init` and `survey_add_definition` functions to support lazy loading.
- Added new methods: `plot.SurveyQuestion`, `get_ggplot`, and `get_echarts` for on-demand plot generation.
- Created comprehensive tests to validate lazy loading behavior and performance improvements.
- Updated documentation for new methods and functionalities.
- Modified existing test scripts to ensure compatibility with lazy loading features.
</commit_message>
<xml_diff>
--- a/inst/extdata/mock_seged.xlsx
+++ b/inst/extdata/mock_seged.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbali\Documents\Projektek\custom_packages\rflib\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81AA011C-19BA-4FC2-ACBA-A667A6A8A49D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A4B3A14-A661-4E27-83D5-431E6EEA7BD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{912F9847-1AF1-481B-9E06-52B0F0841963}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{912F9847-1AF1-481B-9E06-52B0F0841963}"/>
   </bookViews>
   <sheets>
     <sheet name="Types" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="35">
   <si>
     <t>kerdes_szam</t>
   </si>
@@ -141,6 +141,9 @@
   </si>
   <si>
     <t>group3</t>
+  </si>
+  <si>
+    <t>col_eloszlas_total</t>
   </si>
 </sst>
 </file>
@@ -521,7 +524,9 @@
   <sheetPr codeName="Munka1"/>
   <dimension ref="A1:D39"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -592,7 +597,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>34</v>
       </c>
       <c r="C6" s="1">
         <v>1</v>
@@ -603,7 +608,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>34</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -875,7 +880,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{662A3F05-A97A-4276-B2AE-1E6E7FF6A7AA}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>

</xml_diff>